<commit_message>
updating CRS and SRS
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/CRS.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/CRS.xlsx
@@ -177,7 +177,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,6 +353,39 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -391,67 +424,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -772,150 +772,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
       <c r="D1" s="11"/>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="22.5" customHeight="1" thickTop="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="35" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="35" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="16"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="16"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" ht="15.75">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="16"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="17"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="16"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="16"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="46"/>
+      <c r="C11" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="16"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="17"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="16"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" spans="1:5" ht="121.5" customHeight="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="48" t="s">
+      <c r="A13" s="28"/>
+      <c r="B13" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="16"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="16"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A15" s="23"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="24"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="13" t="s">
@@ -931,17 +931,17 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3"/>
-      <c r="B18" s="40"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="4"/>
-      <c r="B19" s="41"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4"/>
-      <c r="B20" s="41"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="5"/>
     </row>
   </sheetData>
@@ -993,92 +993,92 @@
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="54" customHeight="1">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="39" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="29"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="8"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="29"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="8"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="29"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="8"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="39" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="29"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="8"/>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="29"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="8"/>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A9" s="29"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="8"/>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="29"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="8"/>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="29"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="8"/>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="28.5" customHeight="1">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" ht="75" customHeight="1">
-      <c r="A13" s="23"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="24"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
     </row>

</xml_diff>